<commit_message>
Group 6 Estimated Effort spreadsheet update
</commit_message>
<xml_diff>
--- a/Group 6 Estimated Effort.xlsx
+++ b/Group 6 Estimated Effort.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
   <si>
     <t>Task Name: (Dependencies top to bottom)</t>
   </si>
@@ -95,16 +95,16 @@
     <t>Project Manager</t>
   </si>
   <si>
+    <t>Hamza</t>
+  </si>
+  <si>
     <t>Requirements</t>
   </si>
   <si>
-    <t>Gather</t>
+    <t>Analyze</t>
   </si>
   <si>
     <t>Requirements Engineer</t>
-  </si>
-  <si>
-    <t>Analyze</t>
   </si>
   <si>
     <r>
@@ -121,6 +121,9 @@
     <t>Specify</t>
   </si>
   <si>
+    <t>Joel, Jacob, Hamza, Kris, Min, Adrian</t>
+  </si>
+  <si>
     <t>Documentation</t>
   </si>
   <si>
@@ -153,24 +156,6 @@
     <t>Project Manager, Developers</t>
   </si>
   <si>
-    <t>Architecture Document</t>
-  </si>
-  <si>
-    <t>Architect</t>
-  </si>
-  <si>
-    <t>Test Report</t>
-  </si>
-  <si>
-    <t>Tester</t>
-  </si>
-  <si>
-    <t>User Guide &amp; System Admin Doc</t>
-  </si>
-  <si>
-    <t>Developers, Requirements Engineer</t>
-  </si>
-  <si>
     <t>Coding</t>
   </si>
   <si>
@@ -189,10 +174,7 @@
     <t>Research and learn new language and environment</t>
   </si>
   <si>
-    <t>Joel, Jacob, Hamza, Kris, Min, Adrian</t>
-  </si>
-  <si>
-    <t>Set up basic HTML/CSS for web pages</t>
+    <t>Set up log in page (front end)</t>
   </si>
   <si>
     <r>
@@ -205,22 +187,58 @@
     </r>
   </si>
   <si>
-    <t>Write basic SQL queries</t>
-  </si>
-  <si>
-    <t>Min</t>
+    <t>Set up home page for user (front end)</t>
+  </si>
+  <si>
+    <t>Joel, Jacob</t>
+  </si>
+  <si>
+    <t>Set up home page for admin (front end)</t>
+  </si>
+  <si>
+    <t>Database ER diagram</t>
+  </si>
+  <si>
+    <t>Kris, Min</t>
+  </si>
+  <si>
+    <t>Set up database/tables</t>
+  </si>
+  <si>
+    <t>Insert data for user and admin</t>
+  </si>
+  <si>
+    <t>Insert data for streaming services</t>
+  </si>
+  <si>
+    <t>Insert data for TV Shows</t>
   </si>
   <si>
     <t>Implement classes</t>
   </si>
   <si>
+    <t>Hamza, Adrian</t>
+  </si>
+  <si>
+    <t>Set up database connection</t>
+  </si>
+  <si>
+    <t>Set up functionality for login page</t>
+  </si>
+  <si>
     <t>Analysis</t>
   </si>
   <si>
     <t>System Testing</t>
   </si>
   <si>
-    <t>Bug fix as required</t>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Joel, Jacob, Kris</t>
+  </si>
+  <si>
+    <t>Debug</t>
   </si>
   <si>
     <t>Tester, Developer</t>
@@ -618,7 +636,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -775,17 +793,83 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="4" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="4" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="4" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="4" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="4" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="4" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -796,7 +880,7 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -811,83 +895,8 @@
     <xf numFmtId="59" fontId="4" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="4" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="4" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="4" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="4" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
@@ -907,12 +916,21 @@
     <xf numFmtId="1" fontId="5" fillId="6" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="0" fillId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -946,7 +964,7 @@
     <xf numFmtId="49" fontId="4" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -985,22 +1003,13 @@
     <xf numFmtId="1" fontId="3" fillId="6" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1019,6 +1028,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="0" fillId="5" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2504,7 +2516,9 @@
       <c r="D7" t="s" s="51">
         <v>18</v>
       </c>
-      <c r="E7" s="52"/>
+      <c r="E7" t="s" s="52">
+        <v>19</v>
+      </c>
       <c r="F7" s="53">
         <v>12</v>
       </c>
@@ -2547,30 +2561,30 @@
     </row>
     <row r="8" ht="17" customHeight="1">
       <c r="A8" s="48"/>
-      <c r="B8" t="s" s="37">
-        <v>19</v>
-      </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="42">
-        <f>SUM(F9:F11)</f>
-        <v>9</v>
-      </c>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42">
-        <f>SUM(H9:H11)</f>
-        <v>9</v>
+      <c r="B8" t="s" s="54">
+        <v>20</v>
+      </c>
+      <c r="C8" s="55"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59">
+        <f>SUM(F9:F10)</f>
+        <v>10</v>
+      </c>
+      <c r="H8" s="58"/>
+      <c r="I8" s="59">
+        <f>SUM(H9:H10)</f>
+        <v>6</v>
       </c>
       <c r="J8" s="43"/>
       <c r="K8" s="4"/>
       <c r="L8" s="44"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="46">
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="61">
         <f>SUM(M8:P8)</f>
         <v>0</v>
       </c>
@@ -2592,35 +2606,39 @@
     </row>
     <row r="9" ht="17" customHeight="1">
       <c r="A9" s="48"/>
-      <c r="B9" s="56"/>
-      <c r="C9" t="s" s="57">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s" s="58">
+      <c r="B9" s="62"/>
+      <c r="C9" t="s" s="63">
         <v>21</v>
       </c>
-      <c r="E9" s="59"/>
-      <c r="F9" s="60">
-        <v>2</v>
-      </c>
-      <c r="G9" s="61"/>
-      <c r="H9" s="60">
+      <c r="D9" t="s" s="64">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s" s="65">
+        <v>23</v>
+      </c>
+      <c r="F9" s="66">
+        <v>4</v>
+      </c>
+      <c r="G9" s="67">
+        <v>8</v>
+      </c>
+      <c r="H9" s="66">
         <f>SUM(M9:P9)</f>
         <v>3</v>
       </c>
-      <c r="I9" s="61"/>
+      <c r="I9" s="67"/>
       <c r="J9" s="43"/>
       <c r="K9" s="4"/>
       <c r="L9" s="44"/>
-      <c r="M9" s="62">
+      <c r="M9" s="68">
         <v>2</v>
       </c>
-      <c r="N9" s="62">
+      <c r="N9" s="68">
         <v>1</v>
       </c>
-      <c r="O9" s="62"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="63">
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="69">
         <f>SUM(M9:P9)</f>
         <v>3</v>
       </c>
@@ -2640,41 +2658,41 @@
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" ht="31" customHeight="1">
       <c r="A10" s="48"/>
-      <c r="B10" s="64"/>
-      <c r="C10" t="s" s="65">
+      <c r="B10" s="70"/>
+      <c r="C10" t="s" s="71">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s" s="72">
         <v>22</v>
       </c>
-      <c r="D10" t="s" s="66">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s" s="67">
-        <v>23</v>
-      </c>
-      <c r="F10" s="68">
-        <v>4</v>
-      </c>
-      <c r="G10" s="69">
-        <v>5</v>
-      </c>
-      <c r="H10" s="68">
+      <c r="E10" t="s" s="73">
+        <v>25</v>
+      </c>
+      <c r="F10" s="74">
+        <v>6</v>
+      </c>
+      <c r="G10" s="75">
+        <v>12</v>
+      </c>
+      <c r="H10" s="74">
         <f>SUM(M10:P10)</f>
         <v>3</v>
       </c>
-      <c r="I10" s="69"/>
+      <c r="I10" s="75"/>
       <c r="J10" s="43"/>
       <c r="K10" s="4"/>
       <c r="L10" s="44"/>
-      <c r="M10" s="70">
+      <c r="M10" s="76">
+        <v>1</v>
+      </c>
+      <c r="N10" s="76">
         <v>2</v>
       </c>
-      <c r="N10" s="70">
-        <v>1</v>
-      </c>
-      <c r="O10" s="70"/>
-      <c r="P10" s="70"/>
-      <c r="Q10" s="71">
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="77">
         <f>SUM(M10:P10)</f>
         <v>3</v>
       </c>
@@ -2696,37 +2714,32 @@
     </row>
     <row r="11" ht="17" customHeight="1">
       <c r="A11" s="48"/>
-      <c r="B11" s="72"/>
-      <c r="C11" t="s" s="73">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s" s="74">
+      <c r="B11" t="s" s="37">
+        <v>26</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="42">
+        <f>SUM(F12:F15)</f>
+        <v>14</v>
+      </c>
+      <c r="H11" s="41"/>
+      <c r="I11" s="42">
+        <f>SUM(H12:H15)</f>
         <v>21</v>
       </c>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76">
-        <v>3</v>
-      </c>
-      <c r="G11" s="77"/>
-      <c r="H11" s="76">
-        <f>SUM(M11:P11)</f>
-        <v>3</v>
-      </c>
-      <c r="I11" s="77"/>
       <c r="J11" s="43"/>
       <c r="K11" s="4"/>
       <c r="L11" s="44"/>
-      <c r="M11" s="78">
-        <v>1</v>
-      </c>
-      <c r="N11" s="78">
-        <v>2</v>
-      </c>
-      <c r="O11" s="78"/>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="79">
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="45"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="46">
         <f>SUM(M11:P11)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R11" s="47"/>
       <c r="S11" s="4"/>
@@ -2746,32 +2759,41 @@
     </row>
     <row r="12" ht="17" customHeight="1">
       <c r="A12" s="48"/>
-      <c r="B12" t="s" s="37">
-        <v>25</v>
-      </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="42">
-        <f>SUM(F13:F19)</f>
-        <v>28</v>
-      </c>
-      <c r="H12" s="41"/>
-      <c r="I12" s="42">
-        <f>SUM(H13:H19)</f>
-        <v>38.5</v>
-      </c>
+      <c r="B12" s="78"/>
+      <c r="C12" t="s" s="79">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s" s="80">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s" s="81">
+        <v>23</v>
+      </c>
+      <c r="F12" s="82">
+        <v>2</v>
+      </c>
+      <c r="G12" s="83">
+        <v>6</v>
+      </c>
+      <c r="H12" s="82">
+        <f>SUM(M12:P12)</f>
+        <v>3</v>
+      </c>
+      <c r="I12" s="83"/>
       <c r="J12" s="43"/>
       <c r="K12" s="4"/>
       <c r="L12" s="44"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="46">
+      <c r="M12" s="84">
+        <v>0</v>
+      </c>
+      <c r="N12" s="84">
+        <v>3</v>
+      </c>
+      <c r="O12" s="84"/>
+      <c r="P12" s="84"/>
+      <c r="Q12" s="85">
         <f>SUM(M12:P12)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R12" s="47"/>
       <c r="S12" s="4"/>
@@ -2789,43 +2811,41 @@
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
     </row>
-    <row r="13" ht="17" customHeight="1">
+    <row r="13" ht="31" customHeight="1">
       <c r="A13" s="48"/>
-      <c r="B13" s="56"/>
-      <c r="C13" t="s" s="57">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s" s="58">
+      <c r="B13" s="62"/>
+      <c r="C13" t="s" s="63">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s" s="64">
         <v>18</v>
       </c>
-      <c r="E13" t="s" s="80">
-        <v>23</v>
-      </c>
-      <c r="F13" s="60">
+      <c r="E13" t="s" s="65">
+        <v>25</v>
+      </c>
+      <c r="F13" s="66">
         <v>2</v>
       </c>
-      <c r="G13" s="61">
-        <v>6</v>
-      </c>
-      <c r="H13" s="60">
+      <c r="G13" s="67"/>
+      <c r="H13" s="66">
         <f>SUM(M13:P13)</f>
-        <v>3</v>
-      </c>
-      <c r="I13" s="61"/>
+        <v>3.5</v>
+      </c>
+      <c r="I13" s="67"/>
       <c r="J13" s="43"/>
       <c r="K13" s="4"/>
       <c r="L13" s="44"/>
-      <c r="M13" s="62">
-        <v>0</v>
-      </c>
-      <c r="N13" s="62">
+      <c r="M13" s="68">
+        <v>0.5</v>
+      </c>
+      <c r="N13" s="68">
         <v>3</v>
       </c>
-      <c r="O13" s="62"/>
-      <c r="P13" s="62"/>
-      <c r="Q13" s="63">
+      <c r="O13" s="68"/>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="69">
         <f>SUM(M13:P13)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="R13" s="47"/>
       <c r="S13" s="4"/>
@@ -2843,39 +2863,43 @@
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
     </row>
-    <row r="14" ht="17" customHeight="1">
+    <row r="14" ht="31" customHeight="1">
       <c r="A14" s="48"/>
-      <c r="B14" s="64"/>
-      <c r="C14" t="s" s="65">
-        <v>27</v>
-      </c>
-      <c r="D14" t="s" s="66">
+      <c r="B14" s="62"/>
+      <c r="C14" t="s" s="63">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s" s="64">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s" s="65">
+        <v>31</v>
+      </c>
+      <c r="F14" s="66">
+        <v>5</v>
+      </c>
+      <c r="G14" s="67">
         <v>18</v>
       </c>
-      <c r="E14" s="81"/>
-      <c r="F14" s="68">
-        <v>2</v>
-      </c>
-      <c r="G14" s="69"/>
-      <c r="H14" s="68">
+      <c r="H14" s="66">
         <f>SUM(M14:P14)</f>
-        <v>3.5</v>
-      </c>
-      <c r="I14" s="69"/>
+        <v>6.5</v>
+      </c>
+      <c r="I14" s="67"/>
       <c r="J14" s="43"/>
       <c r="K14" s="4"/>
       <c r="L14" s="44"/>
-      <c r="M14" s="70">
+      <c r="M14" s="68">
         <v>0.5</v>
       </c>
-      <c r="N14" s="70">
-        <v>3</v>
-      </c>
-      <c r="O14" s="70"/>
-      <c r="P14" s="70"/>
-      <c r="Q14" s="71">
+      <c r="N14" s="68">
+        <v>6</v>
+      </c>
+      <c r="O14" s="68"/>
+      <c r="P14" s="68"/>
+      <c r="Q14" s="69">
         <f>SUM(M14:P14)</f>
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="R14" s="47"/>
       <c r="S14" s="4"/>
@@ -2894,42 +2918,42 @@
       <c r="AF14" s="4"/>
     </row>
     <row r="15" ht="31" customHeight="1">
-      <c r="A15" s="48"/>
-      <c r="B15" s="64"/>
-      <c r="C15" t="s" s="65">
-        <v>28</v>
-      </c>
-      <c r="D15" t="s" s="66">
-        <v>29</v>
-      </c>
-      <c r="E15" t="s" s="67">
-        <v>30</v>
-      </c>
-      <c r="F15" s="68">
+      <c r="A15" s="86"/>
+      <c r="B15" s="70"/>
+      <c r="C15" t="s" s="71">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s" s="72">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s" s="73">
+        <v>25</v>
+      </c>
+      <c r="F15" s="74">
         <v>5</v>
       </c>
-      <c r="G15" s="69">
+      <c r="G15" s="75"/>
+      <c r="H15" s="74">
+        <f>SUM(M15:P15)</f>
         <v>8</v>
       </c>
-      <c r="H15" s="68">
-        <f>SUM(M15:P15)</f>
-        <v>6.5</v>
-      </c>
-      <c r="I15" s="69"/>
+      <c r="I15" s="75"/>
       <c r="J15" s="43"/>
       <c r="K15" s="4"/>
       <c r="L15" s="44"/>
-      <c r="M15" s="70">
-        <v>0.5</v>
-      </c>
-      <c r="N15" s="70">
+      <c r="M15" s="76">
+        <v>0</v>
+      </c>
+      <c r="N15" s="76">
         <v>6</v>
       </c>
-      <c r="O15" s="70"/>
-      <c r="P15" s="70"/>
-      <c r="Q15" s="71">
+      <c r="O15" s="76"/>
+      <c r="P15" s="76">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="77">
         <f>SUM(M15:P15)</f>
-        <v>6.5</v>
+        <v>8</v>
       </c>
       <c r="R15" s="47"/>
       <c r="S15" s="4"/>
@@ -2947,1050 +2971,1056 @@
       <c r="AE15" s="4"/>
       <c r="AF15" s="4"/>
     </row>
-    <row r="16" ht="31" customHeight="1">
-      <c r="A16" s="48"/>
-      <c r="B16" s="64"/>
-      <c r="C16" t="s" s="65">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s" s="66">
-        <v>32</v>
-      </c>
-      <c r="E16" s="81"/>
-      <c r="F16" s="68">
-        <v>5</v>
-      </c>
-      <c r="G16" s="69"/>
-      <c r="H16" s="68">
+    <row r="16" ht="17" customHeight="1">
+      <c r="A16" t="s" s="87">
+        <v>34</v>
+      </c>
+      <c r="B16" s="88"/>
+      <c r="C16" s="88"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="91"/>
+      <c r="H16" s="90">
         <f>SUM(M16:P16)</f>
-        <v>8</v>
-      </c>
-      <c r="I16" s="69"/>
-      <c r="J16" s="43"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="70">
         <v>0</v>
       </c>
-      <c r="N16" s="70">
-        <v>6</v>
-      </c>
-      <c r="O16" s="70"/>
-      <c r="P16" s="70">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="71">
+      <c r="I16" s="92"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="95"/>
+      <c r="M16" s="96"/>
+      <c r="N16" s="96"/>
+      <c r="O16" s="96"/>
+      <c r="P16" s="96"/>
+      <c r="Q16" s="96">
         <f>SUM(M16:P16)</f>
-        <v>8</v>
-      </c>
-      <c r="R16" s="47"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
-      <c r="AA16" s="4"/>
-      <c r="AB16" s="4"/>
-      <c r="AC16" s="4"/>
-      <c r="AD16" s="4"/>
-      <c r="AE16" s="4"/>
-      <c r="AF16" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="97"/>
+      <c r="S16" s="94"/>
+      <c r="T16" s="94"/>
+      <c r="U16" s="94"/>
+      <c r="V16" s="94"/>
+      <c r="W16" s="94"/>
+      <c r="X16" s="94"/>
+      <c r="Y16" s="94"/>
+      <c r="Z16" s="94"/>
+      <c r="AA16" s="94"/>
+      <c r="AB16" s="94"/>
+      <c r="AC16" s="94"/>
+      <c r="AD16" s="94"/>
+      <c r="AE16" s="94"/>
+      <c r="AF16" s="94"/>
     </row>
     <row r="17" ht="17" customHeight="1">
-      <c r="A17" s="48"/>
-      <c r="B17" s="64"/>
-      <c r="C17" t="s" s="65">
-        <v>33</v>
-      </c>
-      <c r="D17" t="s" s="66">
-        <v>34</v>
-      </c>
-      <c r="E17" s="81"/>
-      <c r="F17" s="68">
-        <v>4</v>
-      </c>
-      <c r="G17" s="69"/>
-      <c r="H17" s="68">
+      <c r="A17" t="s" s="98">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s" s="99">
+        <v>36</v>
+      </c>
+      <c r="C17" s="100"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="42">
+        <f>SUM(F18:F26)</f>
+        <v>98</v>
+      </c>
+      <c r="H17" s="102"/>
+      <c r="I17" s="42">
+        <f>SUM(H18:H26)</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="103"/>
+      <c r="M17" s="104"/>
+      <c r="N17" s="104"/>
+      <c r="O17" s="104"/>
+      <c r="P17" s="104"/>
+      <c r="Q17" s="104">
         <f>SUM(M17:P17)</f>
-        <v>4</v>
-      </c>
-      <c r="I17" s="69"/>
-      <c r="J17" s="43"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="70">
+        <v>0</v>
+      </c>
+      <c r="R17" s="21"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="5"/>
+      <c r="AB17" s="5"/>
+      <c r="AC17" s="5"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+    </row>
+    <row r="18" ht="31" customHeight="1">
+      <c r="A18" s="105"/>
+      <c r="B18" s="106"/>
+      <c r="C18" t="s" s="107">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s" s="108">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s" s="109">
+        <v>25</v>
+      </c>
+      <c r="F18" s="110">
+        <v>6</v>
+      </c>
+      <c r="G18" s="111"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="103"/>
+      <c r="M18" s="113"/>
+      <c r="N18" s="113"/>
+      <c r="O18" s="113">
+        <v>1</v>
+      </c>
+      <c r="P18" s="113">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="113">
+        <f>SUM(M18:P18)</f>
         <v>2</v>
       </c>
-      <c r="N17" s="70">
-        <v>2</v>
-      </c>
-      <c r="O17" s="70"/>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="71">
-        <f>SUM(M17:P17)</f>
-        <v>4</v>
-      </c>
-      <c r="R17" s="47"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
-      <c r="AA17" s="4"/>
-      <c r="AB17" s="4"/>
-      <c r="AC17" s="4"/>
-      <c r="AD17" s="4"/>
-      <c r="AE17" s="4"/>
-      <c r="AF17" s="4"/>
-    </row>
-    <row r="18" ht="17" customHeight="1">
-      <c r="A18" s="48"/>
-      <c r="B18" s="64"/>
-      <c r="C18" t="s" s="65">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s" s="66">
-        <v>36</v>
-      </c>
-      <c r="E18" s="81"/>
-      <c r="F18" s="68">
-        <v>8</v>
-      </c>
-      <c r="G18" s="69"/>
-      <c r="H18" s="68">
-        <f>SUM(M18:P18)</f>
-        <v>7</v>
-      </c>
-      <c r="I18" s="69"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="70">
-        <v>1</v>
-      </c>
-      <c r="N18" s="70">
-        <v>6</v>
-      </c>
-      <c r="O18" s="70"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="71">
-        <f>SUM(M18:P18)</f>
-        <v>7</v>
-      </c>
-      <c r="R18" s="47"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
-      <c r="AA18" s="4"/>
-      <c r="AB18" s="4"/>
-      <c r="AC18" s="4"/>
-      <c r="AD18" s="4"/>
-      <c r="AE18" s="4"/>
-      <c r="AF18" s="4"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="5"/>
     </row>
     <row r="19" ht="31" customHeight="1">
-      <c r="A19" s="82"/>
-      <c r="B19" s="83"/>
-      <c r="C19" t="s" s="73">
-        <v>37</v>
-      </c>
-      <c r="D19" t="s" s="73">
+      <c r="A19" s="105"/>
+      <c r="B19" s="114"/>
+      <c r="C19" t="s" s="115">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s" s="115">
         <v>38</v>
       </c>
-      <c r="E19" s="75"/>
-      <c r="F19" s="83">
-        <v>2</v>
-      </c>
-      <c r="G19" s="84"/>
-      <c r="H19" s="83">
+      <c r="E19" t="s" s="116">
+        <v>25</v>
+      </c>
+      <c r="F19" s="117">
+        <v>24</v>
+      </c>
+      <c r="G19" s="118"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="94"/>
+      <c r="L19" s="95"/>
+      <c r="M19" s="119">
+        <v>1</v>
+      </c>
+      <c r="N19" s="119"/>
+      <c r="O19" s="119">
+        <v>22</v>
+      </c>
+      <c r="P19" s="119">
+        <v>9</v>
+      </c>
+      <c r="Q19" s="119">
         <f>SUM(M19:P19)</f>
-        <v>6.5</v>
-      </c>
-      <c r="I19" s="77"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="86"/>
-      <c r="L19" s="87"/>
-      <c r="M19" s="78">
-        <v>0.5</v>
-      </c>
-      <c r="N19" s="78">
-        <v>5</v>
-      </c>
-      <c r="O19" s="78"/>
-      <c r="P19" s="78">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="88">
-        <f>SUM(M19:P19)</f>
-        <v>6.5</v>
-      </c>
-      <c r="R19" s="89"/>
-      <c r="S19" s="86"/>
-      <c r="T19" s="86"/>
-      <c r="U19" s="86"/>
-      <c r="V19" s="86"/>
-      <c r="W19" s="86"/>
-      <c r="X19" s="86"/>
-      <c r="Y19" s="86"/>
-      <c r="Z19" s="86"/>
-      <c r="AA19" s="86"/>
-      <c r="AB19" s="86"/>
-      <c r="AC19" s="86"/>
-      <c r="AD19" s="86"/>
-      <c r="AE19" s="86"/>
-      <c r="AF19" s="86"/>
+        <v>32</v>
+      </c>
+      <c r="R19" s="97"/>
+      <c r="S19" s="94"/>
+      <c r="T19" s="94"/>
+      <c r="U19" s="94"/>
+      <c r="V19" s="94"/>
+      <c r="W19" s="94"/>
+      <c r="X19" s="94"/>
+      <c r="Y19" s="94"/>
+      <c r="Z19" s="94"/>
+      <c r="AA19" s="94"/>
+      <c r="AB19" s="94"/>
+      <c r="AC19" s="94"/>
+      <c r="AD19" s="94"/>
+      <c r="AE19" s="94"/>
+      <c r="AF19" s="94"/>
     </row>
     <row r="20" ht="17" customHeight="1">
-      <c r="A20" t="s" s="90">
-        <v>39</v>
-      </c>
-      <c r="B20" s="91"/>
-      <c r="C20" s="91"/>
-      <c r="D20" s="91"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="93"/>
-      <c r="G20" s="94"/>
-      <c r="H20" s="93">
+      <c r="A20" s="105"/>
+      <c r="B20" s="114"/>
+      <c r="C20" t="s" s="115">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s" s="115">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s" s="120">
+        <v>41</v>
+      </c>
+      <c r="F20" s="117">
+        <v>14</v>
+      </c>
+      <c r="G20" s="118"/>
+      <c r="H20" s="117"/>
+      <c r="I20" s="118"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="95"/>
+      <c r="M20" s="119">
+        <v>5</v>
+      </c>
+      <c r="N20" s="119"/>
+      <c r="O20" s="119"/>
+      <c r="P20" s="119"/>
+      <c r="Q20" s="119">
         <f>SUM(M20:P20)</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="95"/>
-      <c r="J20" s="85"/>
-      <c r="K20" s="86"/>
-      <c r="L20" s="96"/>
-      <c r="M20" s="97"/>
-      <c r="N20" s="97"/>
-      <c r="O20" s="97"/>
-      <c r="P20" s="97"/>
-      <c r="Q20" s="97">
-        <f>SUM(M20:P20)</f>
-        <v>0</v>
-      </c>
-      <c r="R20" s="89"/>
-      <c r="S20" s="86"/>
-      <c r="T20" s="86"/>
-      <c r="U20" s="86"/>
-      <c r="V20" s="86"/>
-      <c r="W20" s="86"/>
-      <c r="X20" s="86"/>
-      <c r="Y20" s="86"/>
-      <c r="Z20" s="86"/>
-      <c r="AA20" s="86"/>
-      <c r="AB20" s="86"/>
-      <c r="AC20" s="86"/>
-      <c r="AD20" s="86"/>
-      <c r="AE20" s="86"/>
-      <c r="AF20" s="86"/>
+        <v>5</v>
+      </c>
+      <c r="R20" s="97"/>
+      <c r="S20" s="94"/>
+      <c r="T20" s="94"/>
+      <c r="U20" s="94"/>
+      <c r="V20" s="94"/>
+      <c r="W20" s="94"/>
+      <c r="X20" s="94"/>
+      <c r="Y20" s="94"/>
+      <c r="Z20" s="94"/>
+      <c r="AA20" s="94"/>
+      <c r="AB20" s="94"/>
+      <c r="AC20" s="94"/>
+      <c r="AD20" s="94"/>
+      <c r="AE20" s="94"/>
+      <c r="AF20" s="94"/>
     </row>
     <row r="21" ht="17" customHeight="1">
-      <c r="A21" t="s" s="98">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s" s="99">
-        <v>41</v>
-      </c>
-      <c r="C21" s="100"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="102"/>
-      <c r="G21" s="42">
-        <f>SUM(F22:F30)</f>
-        <v>55</v>
-      </c>
-      <c r="H21" s="102"/>
-      <c r="I21" s="42">
-        <f>SUM(H22:H30)</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="103"/>
-      <c r="M21" s="104"/>
-      <c r="N21" s="104"/>
-      <c r="O21" s="104"/>
-      <c r="P21" s="104"/>
-      <c r="Q21" s="104">
+      <c r="A21" s="105"/>
+      <c r="B21" s="114"/>
+      <c r="C21" t="s" s="115">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s" s="115">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s" s="120">
+        <v>43</v>
+      </c>
+      <c r="F21" s="117">
+        <v>12</v>
+      </c>
+      <c r="G21" s="118"/>
+      <c r="H21" s="117"/>
+      <c r="I21" s="118"/>
+      <c r="J21" s="93"/>
+      <c r="K21" s="94"/>
+      <c r="L21" s="95"/>
+      <c r="M21" s="119">
+        <v>10</v>
+      </c>
+      <c r="N21" s="119"/>
+      <c r="O21" s="119"/>
+      <c r="P21" s="119"/>
+      <c r="Q21" s="119">
         <f>SUM(M21:P21)</f>
-        <v>0</v>
-      </c>
-      <c r="R21" s="21"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
-      <c r="Y21" s="5"/>
-      <c r="Z21" s="5"/>
-      <c r="AA21" s="5"/>
-      <c r="AB21" s="5"/>
-      <c r="AC21" s="5"/>
-      <c r="AD21" s="5"/>
-      <c r="AE21" s="5"/>
-      <c r="AF21" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="R21" s="97"/>
+      <c r="S21" s="94"/>
+      <c r="T21" s="94"/>
+      <c r="U21" s="94"/>
+      <c r="V21" s="94"/>
+      <c r="W21" s="94"/>
+      <c r="X21" s="94"/>
+      <c r="Y21" s="94"/>
+      <c r="Z21" s="94"/>
+      <c r="AA21" s="94"/>
+      <c r="AB21" s="94"/>
+      <c r="AC21" s="94"/>
+      <c r="AD21" s="94"/>
+      <c r="AE21" s="94"/>
+      <c r="AF21" s="94"/>
     </row>
     <row r="22" ht="17" customHeight="1">
       <c r="A22" s="105"/>
-      <c r="B22" s="106"/>
-      <c r="C22" t="s" s="107">
-        <v>42</v>
-      </c>
-      <c r="D22" t="s" s="108">
+      <c r="B22" s="121"/>
+      <c r="C22" t="s" s="115">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s" s="115">
+        <v>38</v>
+      </c>
+      <c r="E22" t="s" s="116">
         <v>43</v>
       </c>
-      <c r="E22" s="109"/>
-      <c r="F22" s="110">
-        <v>1</v>
-      </c>
-      <c r="G22" s="111"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="112"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="103"/>
-      <c r="M22" s="113"/>
-      <c r="N22" s="113"/>
-      <c r="O22" s="113">
-        <v>1</v>
-      </c>
-      <c r="P22" s="113">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="113">
+      <c r="F22" s="117">
+        <v>10</v>
+      </c>
+      <c r="G22" s="118"/>
+      <c r="H22" s="117"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="93"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="95"/>
+      <c r="M22" s="119"/>
+      <c r="N22" s="119"/>
+      <c r="O22" s="119"/>
+      <c r="P22" s="119">
+        <v>12</v>
+      </c>
+      <c r="Q22" s="119">
         <f>SUM(M22:P22)</f>
-        <v>2</v>
-      </c>
-      <c r="R22" s="21"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-      <c r="U22" s="5"/>
-      <c r="V22" s="5"/>
-      <c r="W22" s="5"/>
-      <c r="X22" s="5"/>
-      <c r="Y22" s="5"/>
-      <c r="Z22" s="5"/>
-      <c r="AA22" s="5"/>
-      <c r="AB22" s="5"/>
-      <c r="AC22" s="5"/>
-      <c r="AD22" s="5"/>
-      <c r="AE22" s="5"/>
-      <c r="AF22" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="R22" s="97"/>
+      <c r="S22" s="94"/>
+      <c r="T22" s="94"/>
+      <c r="U22" s="94"/>
+      <c r="V22" s="94"/>
+      <c r="W22" s="94"/>
+      <c r="X22" s="94"/>
+      <c r="Y22" s="94"/>
+      <c r="Z22" s="94"/>
+      <c r="AA22" s="94"/>
+      <c r="AB22" s="94"/>
+      <c r="AC22" s="94"/>
+      <c r="AD22" s="94"/>
+      <c r="AE22" s="94"/>
+      <c r="AF22" s="94"/>
     </row>
-    <row r="23" ht="31" customHeight="1">
+    <row r="23" ht="17" customHeight="1">
       <c r="A23" s="105"/>
-      <c r="B23" s="114"/>
+      <c r="B23" s="121"/>
       <c r="C23" t="s" s="115">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s" s="115">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E23" t="s" s="116">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F23" s="117">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G23" s="118"/>
       <c r="H23" s="117"/>
       <c r="I23" s="118"/>
-      <c r="J23" s="85"/>
-      <c r="K23" s="86"/>
-      <c r="L23" s="96"/>
-      <c r="M23" s="119">
-        <v>1</v>
-      </c>
+      <c r="J23" s="93"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="119"/>
       <c r="N23" s="119"/>
-      <c r="O23" s="119">
-        <v>22</v>
-      </c>
+      <c r="O23" s="119"/>
       <c r="P23" s="119">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q23" s="119">
         <f>SUM(M23:P23)</f>
-        <v>32</v>
-      </c>
-      <c r="R23" s="89"/>
-      <c r="S23" s="86"/>
-      <c r="T23" s="86"/>
-      <c r="U23" s="86"/>
-      <c r="V23" s="86"/>
-      <c r="W23" s="86"/>
-      <c r="X23" s="86"/>
-      <c r="Y23" s="86"/>
-      <c r="Z23" s="86"/>
-      <c r="AA23" s="86"/>
-      <c r="AB23" s="86"/>
-      <c r="AC23" s="86"/>
-      <c r="AD23" s="86"/>
-      <c r="AE23" s="86"/>
-      <c r="AF23" s="86"/>
+        <v>5</v>
+      </c>
+      <c r="R23" s="97"/>
+      <c r="S23" s="94"/>
+      <c r="T23" s="94"/>
+      <c r="U23" s="94"/>
+      <c r="V23" s="94"/>
+      <c r="W23" s="94"/>
+      <c r="X23" s="94"/>
+      <c r="Y23" s="94"/>
+      <c r="Z23" s="94"/>
+      <c r="AA23" s="94"/>
+      <c r="AB23" s="94"/>
+      <c r="AC23" s="94"/>
+      <c r="AD23" s="94"/>
+      <c r="AE23" s="94"/>
+      <c r="AF23" s="94"/>
     </row>
     <row r="24" ht="17" customHeight="1">
       <c r="A24" s="105"/>
-      <c r="B24" s="114"/>
+      <c r="B24" s="121"/>
       <c r="C24" t="s" s="115">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s" s="115">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s" s="116">
         <v>46</v>
       </c>
-      <c r="D24" t="s" s="115">
-        <v>43</v>
-      </c>
-      <c r="E24" t="s" s="120">
-        <v>47</v>
-      </c>
       <c r="F24" s="117">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G24" s="118"/>
       <c r="H24" s="117"/>
       <c r="I24" s="118"/>
-      <c r="J24" s="85"/>
-      <c r="K24" s="86"/>
-      <c r="L24" s="96"/>
-      <c r="M24" s="119">
-        <v>5</v>
-      </c>
+      <c r="J24" s="93"/>
+      <c r="K24" s="94"/>
+      <c r="L24" s="95"/>
+      <c r="M24" s="119"/>
       <c r="N24" s="119"/>
       <c r="O24" s="119"/>
-      <c r="P24" s="119"/>
+      <c r="P24" s="119">
+        <v>8</v>
+      </c>
       <c r="Q24" s="119">
         <f>SUM(M24:P24)</f>
-        <v>5</v>
-      </c>
-      <c r="R24" s="89"/>
-      <c r="S24" s="86"/>
-      <c r="T24" s="86"/>
-      <c r="U24" s="86"/>
-      <c r="V24" s="86"/>
-      <c r="W24" s="86"/>
-      <c r="X24" s="86"/>
-      <c r="Y24" s="86"/>
-      <c r="Z24" s="86"/>
-      <c r="AA24" s="86"/>
-      <c r="AB24" s="86"/>
-      <c r="AC24" s="86"/>
-      <c r="AD24" s="86"/>
-      <c r="AE24" s="86"/>
-      <c r="AF24" s="86"/>
+        <v>8</v>
+      </c>
+      <c r="R24" s="97"/>
+      <c r="S24" s="94"/>
+      <c r="T24" s="94"/>
+      <c r="U24" s="94"/>
+      <c r="V24" s="94"/>
+      <c r="W24" s="94"/>
+      <c r="X24" s="94"/>
+      <c r="Y24" s="94"/>
+      <c r="Z24" s="94"/>
+      <c r="AA24" s="94"/>
+      <c r="AB24" s="94"/>
+      <c r="AC24" s="94"/>
+      <c r="AD24" s="94"/>
+      <c r="AE24" s="94"/>
+      <c r="AF24" s="94"/>
     </row>
     <row r="25" ht="17" customHeight="1">
       <c r="A25" s="105"/>
-      <c r="B25" s="114"/>
+      <c r="B25" s="121"/>
       <c r="C25" t="s" s="115">
         <v>48</v>
       </c>
       <c r="D25" t="s" s="115">
-        <v>43</v>
-      </c>
-      <c r="E25" t="s" s="120">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="E25" t="s" s="116">
+        <v>46</v>
       </c>
       <c r="F25" s="117">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G25" s="118"/>
       <c r="H25" s="117"/>
       <c r="I25" s="118"/>
-      <c r="J25" s="85"/>
-      <c r="K25" s="86"/>
-      <c r="L25" s="96"/>
-      <c r="M25" s="119">
-        <v>10</v>
-      </c>
+      <c r="J25" s="93"/>
+      <c r="K25" s="94"/>
+      <c r="L25" s="95"/>
+      <c r="M25" s="119"/>
       <c r="N25" s="119"/>
       <c r="O25" s="119"/>
-      <c r="P25" s="119"/>
+      <c r="P25" s="119">
+        <v>4</v>
+      </c>
       <c r="Q25" s="119">
         <f>SUM(M25:P25)</f>
-        <v>10</v>
-      </c>
-      <c r="R25" s="89"/>
-      <c r="S25" s="86"/>
-      <c r="T25" s="86"/>
-      <c r="U25" s="86"/>
-      <c r="V25" s="86"/>
-      <c r="W25" s="86"/>
-      <c r="X25" s="86"/>
-      <c r="Y25" s="86"/>
-      <c r="Z25" s="86"/>
-      <c r="AA25" s="86"/>
-      <c r="AB25" s="86"/>
-      <c r="AC25" s="86"/>
-      <c r="AD25" s="86"/>
-      <c r="AE25" s="86"/>
-      <c r="AF25" s="86"/>
+        <v>4</v>
+      </c>
+      <c r="R25" s="97"/>
+      <c r="S25" s="94"/>
+      <c r="T25" s="94"/>
+      <c r="U25" s="94"/>
+      <c r="V25" s="94"/>
+      <c r="W25" s="94"/>
+      <c r="X25" s="94"/>
+      <c r="Y25" s="94"/>
+      <c r="Z25" s="94"/>
+      <c r="AA25" s="94"/>
+      <c r="AB25" s="94"/>
+      <c r="AC25" s="94"/>
+      <c r="AD25" s="94"/>
+      <c r="AE25" s="94"/>
+      <c r="AF25" s="94"/>
     </row>
     <row r="26" ht="17" customHeight="1">
       <c r="A26" s="105"/>
       <c r="B26" s="121"/>
       <c r="C26" t="s" s="115">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s" s="115">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E26" t="s" s="116">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F26" s="117">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G26" s="118"/>
       <c r="H26" s="117"/>
       <c r="I26" s="118"/>
-      <c r="J26" s="85"/>
-      <c r="K26" s="86"/>
-      <c r="L26" s="96"/>
+      <c r="J26" s="93"/>
+      <c r="K26" s="94"/>
+      <c r="L26" s="95"/>
       <c r="M26" s="119"/>
       <c r="N26" s="119"/>
       <c r="O26" s="119"/>
-      <c r="P26" s="119">
-        <v>12</v>
-      </c>
+      <c r="P26" s="119"/>
       <c r="Q26" s="119">
         <f>SUM(M26:P26)</f>
-        <v>12</v>
-      </c>
-      <c r="R26" s="89"/>
-      <c r="S26" s="86"/>
-      <c r="T26" s="86"/>
-      <c r="U26" s="86"/>
-      <c r="V26" s="86"/>
-      <c r="W26" s="86"/>
-      <c r="X26" s="86"/>
-      <c r="Y26" s="86"/>
-      <c r="Z26" s="86"/>
-      <c r="AA26" s="86"/>
-      <c r="AB26" s="86"/>
-      <c r="AC26" s="86"/>
-      <c r="AD26" s="86"/>
-      <c r="AE26" s="86"/>
-      <c r="AF26" s="86"/>
+        <v>0</v>
+      </c>
+      <c r="R26" s="97"/>
+      <c r="S26" s="94"/>
+      <c r="T26" s="94"/>
+      <c r="U26" s="94"/>
+      <c r="V26" s="94"/>
+      <c r="W26" s="94"/>
+      <c r="X26" s="94"/>
+      <c r="Y26" s="94"/>
+      <c r="Z26" s="94"/>
+      <c r="AA26" s="94"/>
+      <c r="AB26" s="94"/>
+      <c r="AC26" s="94"/>
+      <c r="AD26" s="94"/>
+      <c r="AE26" s="94"/>
+      <c r="AF26" s="94"/>
     </row>
     <row r="27" ht="17" customHeight="1">
       <c r="A27" s="105"/>
       <c r="B27" s="121"/>
-      <c r="C27" s="122"/>
+      <c r="C27" t="s" s="115">
+        <v>50</v>
+      </c>
       <c r="D27" t="s" s="115">
-        <v>43</v>
-      </c>
-      <c r="E27" s="123"/>
-      <c r="F27" s="117"/>
+        <v>38</v>
+      </c>
+      <c r="E27" t="s" s="116">
+        <v>46</v>
+      </c>
+      <c r="F27" s="117">
+        <v>8</v>
+      </c>
       <c r="G27" s="118"/>
       <c r="H27" s="117"/>
       <c r="I27" s="118"/>
-      <c r="J27" s="85"/>
-      <c r="K27" s="86"/>
-      <c r="L27" s="96"/>
+      <c r="J27" s="93"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="95"/>
       <c r="M27" s="119"/>
       <c r="N27" s="119"/>
       <c r="O27" s="119"/>
-      <c r="P27" s="119">
-        <v>5</v>
-      </c>
+      <c r="P27" s="119"/>
       <c r="Q27" s="119">
         <f>SUM(M27:P27)</f>
-        <v>5</v>
-      </c>
-      <c r="R27" s="89"/>
-      <c r="S27" s="86"/>
-      <c r="T27" s="86"/>
-      <c r="U27" s="86"/>
-      <c r="V27" s="86"/>
-      <c r="W27" s="86"/>
-      <c r="X27" s="86"/>
-      <c r="Y27" s="86"/>
-      <c r="Z27" s="86"/>
-      <c r="AA27" s="86"/>
-      <c r="AB27" s="86"/>
-      <c r="AC27" s="86"/>
-      <c r="AD27" s="86"/>
-      <c r="AE27" s="86"/>
-      <c r="AF27" s="86"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="97"/>
+      <c r="S27" s="94"/>
+      <c r="T27" s="94"/>
+      <c r="U27" s="94"/>
+      <c r="V27" s="94"/>
+      <c r="W27" s="94"/>
+      <c r="X27" s="94"/>
+      <c r="Y27" s="94"/>
+      <c r="Z27" s="94"/>
+      <c r="AA27" s="94"/>
+      <c r="AB27" s="94"/>
+      <c r="AC27" s="94"/>
+      <c r="AD27" s="94"/>
+      <c r="AE27" s="94"/>
+      <c r="AF27" s="94"/>
     </row>
     <row r="28" ht="17" customHeight="1">
       <c r="A28" s="105"/>
       <c r="B28" s="121"/>
-      <c r="C28" s="122"/>
+      <c r="C28" t="s" s="115">
+        <v>51</v>
+      </c>
       <c r="D28" t="s" s="115">
-        <v>43</v>
-      </c>
-      <c r="E28" s="123"/>
-      <c r="F28" s="117"/>
+        <v>38</v>
+      </c>
+      <c r="E28" t="s" s="116">
+        <v>52</v>
+      </c>
+      <c r="F28" s="117">
+        <v>12</v>
+      </c>
       <c r="G28" s="118"/>
       <c r="H28" s="117"/>
       <c r="I28" s="118"/>
-      <c r="J28" s="85"/>
-      <c r="K28" s="86"/>
-      <c r="L28" s="96"/>
+      <c r="J28" s="93"/>
+      <c r="K28" s="94"/>
+      <c r="L28" s="95"/>
       <c r="M28" s="119"/>
       <c r="N28" s="119"/>
       <c r="O28" s="119"/>
-      <c r="P28" s="119">
-        <v>8</v>
-      </c>
+      <c r="P28" s="119"/>
       <c r="Q28" s="119">
         <f>SUM(M28:P28)</f>
-        <v>8</v>
-      </c>
-      <c r="R28" s="89"/>
-      <c r="S28" s="86"/>
-      <c r="T28" s="86"/>
-      <c r="U28" s="86"/>
-      <c r="V28" s="86"/>
-      <c r="W28" s="86"/>
-      <c r="X28" s="86"/>
-      <c r="Y28" s="86"/>
-      <c r="Z28" s="86"/>
-      <c r="AA28" s="86"/>
-      <c r="AB28" s="86"/>
-      <c r="AC28" s="86"/>
-      <c r="AD28" s="86"/>
-      <c r="AE28" s="86"/>
-      <c r="AF28" s="86"/>
+        <v>0</v>
+      </c>
+      <c r="R28" s="97"/>
+      <c r="S28" s="94"/>
+      <c r="T28" s="94"/>
+      <c r="U28" s="94"/>
+      <c r="V28" s="94"/>
+      <c r="W28" s="94"/>
+      <c r="X28" s="94"/>
+      <c r="Y28" s="94"/>
+      <c r="Z28" s="94"/>
+      <c r="AA28" s="94"/>
+      <c r="AB28" s="94"/>
+      <c r="AC28" s="94"/>
+      <c r="AD28" s="94"/>
+      <c r="AE28" s="94"/>
+      <c r="AF28" s="94"/>
     </row>
     <row r="29" ht="17" customHeight="1">
       <c r="A29" s="105"/>
       <c r="B29" s="121"/>
-      <c r="C29" s="122"/>
+      <c r="C29" t="s" s="115">
+        <v>53</v>
+      </c>
       <c r="D29" t="s" s="115">
-        <v>43</v>
-      </c>
-      <c r="E29" s="123"/>
-      <c r="F29" s="117"/>
+        <v>38</v>
+      </c>
+      <c r="E29" t="s" s="116">
+        <v>52</v>
+      </c>
+      <c r="F29" s="117">
+        <v>8</v>
+      </c>
       <c r="G29" s="118"/>
       <c r="H29" s="117"/>
       <c r="I29" s="118"/>
-      <c r="J29" s="85"/>
-      <c r="K29" s="86"/>
-      <c r="L29" s="96"/>
+      <c r="J29" s="93"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="95"/>
       <c r="M29" s="119"/>
       <c r="N29" s="119"/>
       <c r="O29" s="119"/>
-      <c r="P29" s="119">
-        <v>4</v>
-      </c>
+      <c r="P29" s="119"/>
       <c r="Q29" s="119">
         <f>SUM(M29:P29)</f>
-        <v>4</v>
-      </c>
-      <c r="R29" s="89"/>
-      <c r="S29" s="86"/>
-      <c r="T29" s="86"/>
-      <c r="U29" s="86"/>
-      <c r="V29" s="86"/>
-      <c r="W29" s="86"/>
-      <c r="X29" s="86"/>
-      <c r="Y29" s="86"/>
-      <c r="Z29" s="86"/>
-      <c r="AA29" s="86"/>
-      <c r="AB29" s="86"/>
-      <c r="AC29" s="86"/>
-      <c r="AD29" s="86"/>
-      <c r="AE29" s="86"/>
-      <c r="AF29" s="86"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="97"/>
+      <c r="S29" s="94"/>
+      <c r="T29" s="94"/>
+      <c r="U29" s="94"/>
+      <c r="V29" s="94"/>
+      <c r="W29" s="94"/>
+      <c r="X29" s="94"/>
+      <c r="Y29" s="94"/>
+      <c r="Z29" s="94"/>
+      <c r="AA29" s="94"/>
+      <c r="AB29" s="94"/>
+      <c r="AC29" s="94"/>
+      <c r="AD29" s="94"/>
+      <c r="AE29" s="94"/>
+      <c r="AF29" s="94"/>
     </row>
     <row r="30" ht="17" customHeight="1">
       <c r="A30" s="105"/>
-      <c r="B30" s="124"/>
-      <c r="C30" s="125"/>
-      <c r="D30" t="s" s="126">
-        <v>43</v>
-      </c>
-      <c r="E30" s="127"/>
-      <c r="F30" s="128"/>
-      <c r="G30" s="129"/>
-      <c r="H30" s="128"/>
-      <c r="I30" s="129"/>
-      <c r="J30" s="85"/>
-      <c r="K30" s="86"/>
-      <c r="L30" s="96"/>
-      <c r="M30" s="130"/>
-      <c r="N30" s="130"/>
-      <c r="O30" s="130"/>
-      <c r="P30" s="130"/>
-      <c r="Q30" s="130">
+      <c r="B30" s="122"/>
+      <c r="C30" t="s" s="123">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s" s="123">
+        <v>38</v>
+      </c>
+      <c r="E30" t="s" s="124">
+        <v>52</v>
+      </c>
+      <c r="F30" s="125">
+        <v>16</v>
+      </c>
+      <c r="G30" s="126"/>
+      <c r="H30" s="125"/>
+      <c r="I30" s="126"/>
+      <c r="J30" s="93"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="95"/>
+      <c r="M30" s="127"/>
+      <c r="N30" s="127"/>
+      <c r="O30" s="127"/>
+      <c r="P30" s="127"/>
+      <c r="Q30" s="127">
         <f>SUM(M30:P30)</f>
         <v>0</v>
       </c>
-      <c r="R30" s="89"/>
-      <c r="S30" s="86"/>
-      <c r="T30" s="86"/>
-      <c r="U30" s="86"/>
-      <c r="V30" s="86"/>
-      <c r="W30" s="86"/>
-      <c r="X30" s="86"/>
-      <c r="Y30" s="86"/>
-      <c r="Z30" s="86"/>
-      <c r="AA30" s="86"/>
-      <c r="AB30" s="86"/>
-      <c r="AC30" s="86"/>
-      <c r="AD30" s="86"/>
-      <c r="AE30" s="86"/>
-      <c r="AF30" s="86"/>
+      <c r="R30" s="97"/>
+      <c r="S30" s="94"/>
+      <c r="T30" s="94"/>
+      <c r="U30" s="94"/>
+      <c r="V30" s="94"/>
+      <c r="W30" s="94"/>
+      <c r="X30" s="94"/>
+      <c r="Y30" s="94"/>
+      <c r="Z30" s="94"/>
+      <c r="AA30" s="94"/>
+      <c r="AB30" s="94"/>
+      <c r="AC30" s="94"/>
+      <c r="AD30" s="94"/>
+      <c r="AE30" s="94"/>
+      <c r="AF30" s="94"/>
     </row>
     <row r="31" ht="17" customHeight="1">
       <c r="A31" s="105"/>
-      <c r="B31" t="s" s="131">
-        <v>51</v>
-      </c>
-      <c r="C31" s="132"/>
+      <c r="B31" t="s" s="128">
+        <v>55</v>
+      </c>
+      <c r="C31" s="129"/>
       <c r="D31" s="101"/>
       <c r="E31" s="42"/>
       <c r="F31" s="102"/>
-      <c r="G31" s="133">
+      <c r="G31" s="130">
         <f>SUM(F32:F34)</f>
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="H31" s="102"/>
       <c r="I31" s="42">
         <f>SUM(H32:H34)</f>
         <v>0</v>
       </c>
-      <c r="J31" s="85"/>
-      <c r="K31" s="86"/>
-      <c r="L31" s="87"/>
+      <c r="J31" s="93"/>
+      <c r="K31" s="94"/>
+      <c r="L31" s="131"/>
       <c r="M31" s="45"/>
       <c r="N31" s="45"/>
       <c r="O31" s="45"/>
       <c r="P31" s="45"/>
-      <c r="Q31" s="134">
+      <c r="Q31" s="132">
         <f>SUM(M31:P31)</f>
         <v>0</v>
       </c>
-      <c r="R31" s="89"/>
-      <c r="S31" s="86"/>
-      <c r="T31" s="86"/>
-      <c r="U31" s="86"/>
-      <c r="V31" s="86"/>
-      <c r="W31" s="86"/>
-      <c r="X31" s="86"/>
-      <c r="Y31" s="86"/>
-      <c r="Z31" s="86"/>
-      <c r="AA31" s="86"/>
-      <c r="AB31" s="86"/>
-      <c r="AC31" s="86"/>
-      <c r="AD31" s="86"/>
-      <c r="AE31" s="86"/>
-      <c r="AF31" s="86"/>
+      <c r="R31" s="97"/>
+      <c r="S31" s="94"/>
+      <c r="T31" s="94"/>
+      <c r="U31" s="94"/>
+      <c r="V31" s="94"/>
+      <c r="W31" s="94"/>
+      <c r="X31" s="94"/>
+      <c r="Y31" s="94"/>
+      <c r="Z31" s="94"/>
+      <c r="AA31" s="94"/>
+      <c r="AB31" s="94"/>
+      <c r="AC31" s="94"/>
+      <c r="AD31" s="94"/>
+      <c r="AE31" s="94"/>
+      <c r="AF31" s="94"/>
     </row>
     <row r="32" ht="17" customHeight="1">
       <c r="A32" s="105"/>
-      <c r="B32" s="135"/>
-      <c r="C32" t="s" s="136">
-        <v>52</v>
-      </c>
-      <c r="D32" t="s" s="136">
-        <v>36</v>
-      </c>
-      <c r="E32" s="109"/>
-      <c r="F32" s="137">
-        <v>4</v>
+      <c r="B32" s="133"/>
+      <c r="C32" t="s" s="134">
+        <v>56</v>
+      </c>
+      <c r="D32" t="s" s="134">
+        <v>57</v>
+      </c>
+      <c r="E32" t="s" s="109">
+        <v>58</v>
+      </c>
+      <c r="F32" s="135">
+        <v>9</v>
       </c>
       <c r="G32" s="111"/>
-      <c r="H32" s="137"/>
+      <c r="H32" s="135"/>
       <c r="I32" s="111"/>
-      <c r="J32" s="85"/>
-      <c r="K32" s="86"/>
-      <c r="L32" s="87"/>
-      <c r="M32" s="138">
+      <c r="J32" s="93"/>
+      <c r="K32" s="94"/>
+      <c r="L32" s="131"/>
+      <c r="M32" s="136">
         <v>1</v>
       </c>
-      <c r="N32" s="138">
+      <c r="N32" s="136">
         <v>1</v>
       </c>
-      <c r="O32" s="138"/>
-      <c r="P32" s="138"/>
-      <c r="Q32" s="139">
+      <c r="O32" s="136"/>
+      <c r="P32" s="136"/>
+      <c r="Q32" s="137">
         <f>SUM(M32:P32)</f>
         <v>2</v>
       </c>
-      <c r="R32" s="89"/>
-      <c r="S32" s="86"/>
-      <c r="T32" s="86"/>
-      <c r="U32" s="86"/>
-      <c r="V32" s="86"/>
-      <c r="W32" s="86"/>
-      <c r="X32" s="86"/>
-      <c r="Y32" s="86"/>
-      <c r="Z32" s="86"/>
-      <c r="AA32" s="86"/>
-      <c r="AB32" s="86"/>
-      <c r="AC32" s="86"/>
-      <c r="AD32" s="86"/>
-      <c r="AE32" s="86"/>
-      <c r="AF32" s="86"/>
+      <c r="R32" s="97"/>
+      <c r="S32" s="94"/>
+      <c r="T32" s="94"/>
+      <c r="U32" s="94"/>
+      <c r="V32" s="94"/>
+      <c r="W32" s="94"/>
+      <c r="X32" s="94"/>
+      <c r="Y32" s="94"/>
+      <c r="Z32" s="94"/>
+      <c r="AA32" s="94"/>
+      <c r="AB32" s="94"/>
+      <c r="AC32" s="94"/>
+      <c r="AD32" s="94"/>
+      <c r="AE32" s="94"/>
+      <c r="AF32" s="94"/>
     </row>
-    <row r="33" ht="17" customHeight="1">
+    <row r="33" ht="31" customHeight="1">
       <c r="A33" s="105"/>
       <c r="B33" s="121"/>
       <c r="C33" t="s" s="115">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s" s="115">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s" s="120">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="F33" s="117">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G33" s="118"/>
       <c r="H33" s="117"/>
       <c r="I33" s="118"/>
-      <c r="J33" s="85"/>
-      <c r="K33" s="86"/>
-      <c r="L33" s="87"/>
-      <c r="M33" s="140"/>
-      <c r="N33" s="140"/>
-      <c r="O33" s="140"/>
-      <c r="P33" s="140">
+      <c r="J33" s="93"/>
+      <c r="K33" s="94"/>
+      <c r="L33" s="131"/>
+      <c r="M33" s="138"/>
+      <c r="N33" s="138"/>
+      <c r="O33" s="138"/>
+      <c r="P33" s="138">
         <v>1</v>
       </c>
-      <c r="Q33" s="141">
+      <c r="Q33" s="139">
         <f>SUM(M33:P33)</f>
         <v>1</v>
       </c>
-      <c r="R33" s="89"/>
-      <c r="S33" s="86"/>
-      <c r="T33" s="86"/>
-      <c r="U33" s="86"/>
-      <c r="V33" s="86"/>
-      <c r="W33" s="86"/>
-      <c r="X33" s="86"/>
-      <c r="Y33" s="86"/>
-      <c r="Z33" s="86"/>
-      <c r="AA33" s="86"/>
-      <c r="AB33" s="86"/>
-      <c r="AC33" s="86"/>
-      <c r="AD33" s="86"/>
-      <c r="AE33" s="86"/>
-      <c r="AF33" s="86"/>
+      <c r="R33" s="97"/>
+      <c r="S33" s="94"/>
+      <c r="T33" s="94"/>
+      <c r="U33" s="94"/>
+      <c r="V33" s="94"/>
+      <c r="W33" s="94"/>
+      <c r="X33" s="94"/>
+      <c r="Y33" s="94"/>
+      <c r="Z33" s="94"/>
+      <c r="AA33" s="94"/>
+      <c r="AB33" s="94"/>
+      <c r="AC33" s="94"/>
+      <c r="AD33" s="94"/>
+      <c r="AE33" s="94"/>
+      <c r="AF33" s="94"/>
     </row>
     <row r="34" ht="17" customHeight="1">
-      <c r="A34" s="142"/>
-      <c r="B34" s="124"/>
-      <c r="C34" t="s" s="126">
-        <v>55</v>
-      </c>
-      <c r="D34" t="s" s="126">
+      <c r="A34" s="140"/>
+      <c r="B34" s="122"/>
+      <c r="C34" t="s" s="123">
+        <v>61</v>
+      </c>
+      <c r="D34" t="s" s="123">
         <v>18</v>
       </c>
-      <c r="E34" s="127"/>
-      <c r="F34" s="128">
+      <c r="E34" t="s" s="124">
+        <v>19</v>
+      </c>
+      <c r="F34" s="125">
         <v>5</v>
       </c>
-      <c r="G34" s="129"/>
-      <c r="H34" s="128"/>
-      <c r="I34" s="129"/>
-      <c r="J34" s="85"/>
-      <c r="K34" s="86"/>
-      <c r="L34" s="87"/>
-      <c r="M34" s="143">
+      <c r="G34" s="126"/>
+      <c r="H34" s="125"/>
+      <c r="I34" s="126"/>
+      <c r="J34" s="93"/>
+      <c r="K34" s="94"/>
+      <c r="L34" s="131"/>
+      <c r="M34" s="141">
         <v>1</v>
       </c>
-      <c r="N34" s="143">
+      <c r="N34" s="141">
         <v>1</v>
       </c>
-      <c r="O34" s="143"/>
-      <c r="P34" s="143"/>
-      <c r="Q34" s="144">
+      <c r="O34" s="141"/>
+      <c r="P34" s="141"/>
+      <c r="Q34" s="142">
         <f>SUM(M34:P34)</f>
         <v>2</v>
       </c>
-      <c r="R34" s="89"/>
-      <c r="S34" s="86"/>
-      <c r="T34" s="86"/>
-      <c r="U34" s="86"/>
-      <c r="V34" s="86"/>
-      <c r="W34" s="86"/>
-      <c r="X34" s="86"/>
-      <c r="Y34" s="86"/>
-      <c r="Z34" s="86"/>
-      <c r="AA34" s="86"/>
-      <c r="AB34" s="86"/>
-      <c r="AC34" s="86"/>
-      <c r="AD34" s="86"/>
-      <c r="AE34" s="86"/>
-      <c r="AF34" s="86"/>
+      <c r="R34" s="97"/>
+      <c r="S34" s="94"/>
+      <c r="T34" s="94"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="94"/>
+      <c r="W34" s="94"/>
+      <c r="X34" s="94"/>
+      <c r="Y34" s="94"/>
+      <c r="Z34" s="94"/>
+      <c r="AA34" s="94"/>
+      <c r="AB34" s="94"/>
+      <c r="AC34" s="94"/>
+      <c r="AD34" s="94"/>
+      <c r="AE34" s="94"/>
+      <c r="AF34" s="94"/>
     </row>
     <row r="35" ht="13.65" customHeight="1">
-      <c r="A35" t="s" s="145">
+      <c r="A35" t="s" s="143">
         <v>5</v>
       </c>
-      <c r="B35" s="146"/>
-      <c r="C35" s="147"/>
-      <c r="D35" s="147"/>
-      <c r="E35" s="148"/>
-      <c r="F35" s="149">
+      <c r="B35" s="144"/>
+      <c r="C35" s="145"/>
+      <c r="D35" s="145"/>
+      <c r="E35" s="146"/>
+      <c r="F35" s="147">
         <f>SUM(F5:F34)</f>
-        <v>118</v>
-      </c>
-      <c r="G35" s="150">
+        <v>210</v>
+      </c>
+      <c r="G35" s="148">
         <f>SUM(G5:G34)</f>
-        <v>137</v>
-      </c>
-      <c r="H35" s="149">
+        <v>210</v>
+      </c>
+      <c r="H35" s="147">
         <f>SUM(M35:P35)</f>
-        <v>132.5</v>
-      </c>
-      <c r="I35" s="150">
+        <v>112</v>
+      </c>
+      <c r="I35" s="148">
         <f>SUM(I5:I34)</f>
-        <v>49.5</v>
-      </c>
-      <c r="J35" s="85"/>
-      <c r="K35" s="86"/>
-      <c r="L35" s="87"/>
-      <c r="M35" s="151">
+        <v>29</v>
+      </c>
+      <c r="J35" s="93"/>
+      <c r="K35" s="94"/>
+      <c r="L35" s="131"/>
+      <c r="M35" s="149">
         <f>SUM(M5:M34)</f>
-        <v>29.5</v>
-      </c>
-      <c r="N35" s="151">
+        <v>24</v>
+      </c>
+      <c r="N35" s="149">
         <f>SUM(N5:N34)</f>
-        <v>37</v>
-      </c>
-      <c r="O35" s="151">
+        <v>23</v>
+      </c>
+      <c r="O35" s="149">
         <f>SUM(O5:O34)</f>
         <v>23</v>
       </c>
-      <c r="P35" s="151">
+      <c r="P35" s="149">
         <f>SUM(P5:P34)</f>
-        <v>43</v>
-      </c>
-      <c r="Q35" s="152">
+        <v>42</v>
+      </c>
+      <c r="Q35" s="150">
         <f>SUM(M35:P35)</f>
-        <v>132.5</v>
-      </c>
-      <c r="R35" s="89"/>
-      <c r="S35" s="86"/>
-      <c r="T35" s="86"/>
-      <c r="U35" s="86"/>
-      <c r="V35" s="86"/>
-      <c r="W35" s="86"/>
-      <c r="X35" s="86"/>
-      <c r="Y35" s="86"/>
-      <c r="Z35" s="86"/>
-      <c r="AA35" s="86"/>
-      <c r="AB35" s="86"/>
-      <c r="AC35" s="86"/>
-      <c r="AD35" s="86"/>
-      <c r="AE35" s="86"/>
-      <c r="AF35" s="86"/>
+        <v>112</v>
+      </c>
+      <c r="R35" s="97"/>
+      <c r="S35" s="94"/>
+      <c r="T35" s="94"/>
+      <c r="U35" s="94"/>
+      <c r="V35" s="94"/>
+      <c r="W35" s="94"/>
+      <c r="X35" s="94"/>
+      <c r="Y35" s="94"/>
+      <c r="Z35" s="94"/>
+      <c r="AA35" s="94"/>
+      <c r="AB35" s="94"/>
+      <c r="AC35" s="94"/>
+      <c r="AD35" s="94"/>
+      <c r="AE35" s="94"/>
+      <c r="AF35" s="94"/>
     </row>
     <row r="36" ht="13.65" customHeight="1">
-      <c r="A36" s="153"/>
-      <c r="B36" s="153"/>
-      <c r="C36" s="153"/>
-      <c r="D36" s="154"/>
-      <c r="E36" s="153"/>
-      <c r="F36" s="153"/>
-      <c r="G36" s="153"/>
-      <c r="H36" s="153"/>
-      <c r="I36" s="153"/>
-      <c r="J36" s="86"/>
-      <c r="K36" s="86"/>
-      <c r="L36" s="86"/>
-      <c r="M36" s="155"/>
-      <c r="N36" s="155"/>
-      <c r="O36" s="155"/>
-      <c r="P36" s="155"/>
-      <c r="Q36" s="153"/>
-      <c r="R36" s="86"/>
-      <c r="S36" s="86"/>
-      <c r="T36" s="86"/>
-      <c r="U36" s="86"/>
-      <c r="V36" s="86"/>
-      <c r="W36" s="86"/>
-      <c r="X36" s="86"/>
-      <c r="Y36" s="86"/>
-      <c r="Z36" s="86"/>
-      <c r="AA36" s="86"/>
-      <c r="AB36" s="86"/>
-      <c r="AC36" s="86"/>
-      <c r="AD36" s="86"/>
-      <c r="AE36" s="86"/>
-      <c r="AF36" s="86"/>
+      <c r="A36" s="151"/>
+      <c r="B36" s="151"/>
+      <c r="C36" s="151"/>
+      <c r="D36" s="152"/>
+      <c r="E36" s="151"/>
+      <c r="F36" s="151"/>
+      <c r="G36" s="151"/>
+      <c r="H36" s="151"/>
+      <c r="I36" s="151"/>
+      <c r="J36" s="94"/>
+      <c r="K36" s="94"/>
+      <c r="L36" s="94"/>
+      <c r="M36" s="153"/>
+      <c r="N36" s="153"/>
+      <c r="O36" s="153"/>
+      <c r="P36" s="153"/>
+      <c r="Q36" s="151"/>
+      <c r="R36" s="94"/>
+      <c r="S36" s="94"/>
+      <c r="T36" s="94"/>
+      <c r="U36" s="94"/>
+      <c r="V36" s="94"/>
+      <c r="W36" s="94"/>
+      <c r="X36" s="94"/>
+      <c r="Y36" s="94"/>
+      <c r="Z36" s="94"/>
+      <c r="AA36" s="94"/>
+      <c r="AB36" s="94"/>
+      <c r="AC36" s="94"/>
+      <c r="AD36" s="94"/>
+      <c r="AE36" s="94"/>
+      <c r="AF36" s="94"/>
     </row>
     <row r="37" ht="13.65" customHeight="1">
-      <c r="A37" s="86"/>
-      <c r="B37" s="86"/>
-      <c r="C37" s="86"/>
+      <c r="A37" s="94"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="86"/>
-      <c r="H37" s="86"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="86"/>
-      <c r="K37" s="86"/>
-      <c r="L37" s="86"/>
-      <c r="M37" s="156"/>
-      <c r="N37" s="156"/>
-      <c r="O37" s="156"/>
-      <c r="P37" s="156"/>
-      <c r="Q37" s="86"/>
-      <c r="R37" s="86"/>
-      <c r="S37" s="86"/>
-      <c r="T37" s="86"/>
-      <c r="U37" s="86"/>
-      <c r="V37" s="86"/>
-      <c r="W37" s="86"/>
-      <c r="X37" s="86"/>
-      <c r="Y37" s="86"/>
-      <c r="Z37" s="86"/>
-      <c r="AA37" s="86"/>
-      <c r="AB37" s="86"/>
-      <c r="AC37" s="86"/>
-      <c r="AD37" s="86"/>
-      <c r="AE37" s="86"/>
-      <c r="AF37" s="86"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="94"/>
+      <c r="I37" s="94"/>
+      <c r="J37" s="94"/>
+      <c r="K37" s="94"/>
+      <c r="L37" s="94"/>
+      <c r="M37" s="154"/>
+      <c r="N37" s="154"/>
+      <c r="O37" s="154"/>
+      <c r="P37" s="154"/>
+      <c r="Q37" s="94"/>
+      <c r="R37" s="94"/>
+      <c r="S37" s="94"/>
+      <c r="T37" s="94"/>
+      <c r="U37" s="94"/>
+      <c r="V37" s="94"/>
+      <c r="W37" s="94"/>
+      <c r="X37" s="94"/>
+      <c r="Y37" s="94"/>
+      <c r="Z37" s="94"/>
+      <c r="AA37" s="94"/>
+      <c r="AB37" s="94"/>
+      <c r="AC37" s="94"/>
+      <c r="AD37" s="94"/>
+      <c r="AE37" s="94"/>
+      <c r="AF37" s="94"/>
     </row>
     <row r="38" ht="13.65" customHeight="1">
-      <c r="A38" s="86"/>
-      <c r="B38" s="86"/>
-      <c r="C38" s="86"/>
+      <c r="A38" s="94"/>
+      <c r="B38" s="94"/>
+      <c r="C38" s="94"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="86"/>
-      <c r="F38" s="86"/>
-      <c r="G38" s="86"/>
-      <c r="H38" s="86"/>
-      <c r="I38" s="86"/>
-      <c r="J38" s="86"/>
-      <c r="K38" s="86"/>
-      <c r="L38" s="86"/>
-      <c r="M38" s="156"/>
-      <c r="N38" s="156"/>
-      <c r="O38" s="156"/>
-      <c r="P38" s="156"/>
-      <c r="Q38" s="86"/>
-      <c r="R38" s="86"/>
-      <c r="S38" s="86"/>
-      <c r="T38" s="86"/>
-      <c r="U38" s="86"/>
-      <c r="V38" s="86"/>
-      <c r="W38" s="86"/>
-      <c r="X38" s="86"/>
-      <c r="Y38" s="86"/>
-      <c r="Z38" s="86"/>
-      <c r="AA38" s="86"/>
-      <c r="AB38" s="86"/>
-      <c r="AC38" s="86"/>
-      <c r="AD38" s="86"/>
-      <c r="AE38" s="86"/>
-      <c r="AF38" s="86"/>
+      <c r="E38" s="94"/>
+      <c r="F38" s="94"/>
+      <c r="G38" s="94"/>
+      <c r="H38" s="94"/>
+      <c r="I38" s="94"/>
+      <c r="J38" s="94"/>
+      <c r="K38" s="94"/>
+      <c r="L38" s="94"/>
+      <c r="M38" s="154"/>
+      <c r="N38" s="154"/>
+      <c r="O38" s="154"/>
+      <c r="P38" s="154"/>
+      <c r="Q38" s="94"/>
+      <c r="R38" s="94"/>
+      <c r="S38" s="94"/>
+      <c r="T38" s="94"/>
+      <c r="U38" s="94"/>
+      <c r="V38" s="94"/>
+      <c r="W38" s="94"/>
+      <c r="X38" s="94"/>
+      <c r="Y38" s="94"/>
+      <c r="Z38" s="94"/>
+      <c r="AA38" s="94"/>
+      <c r="AB38" s="94"/>
+      <c r="AC38" s="94"/>
+      <c r="AD38" s="94"/>
+      <c r="AE38" s="94"/>
+      <c r="AF38" s="94"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>

</xml_diff>